<commit_message>
chua code dc gi
</commit_message>
<xml_diff>
--- a/src/main/resources/fileTemplate/templatePhieuBienNhan.xlsx
+++ b/src/main/resources/fileTemplate/templatePhieuBienNhan.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="72">
   <si>
     <t>TT</t>
   </si>
@@ -313,9 +313,6 @@
     <t>PHIẾU BIÊN NHẬN</t>
   </si>
   <si>
-    <t>Nhà xe:</t>
-  </si>
-  <si>
     <t>Số biên nhận</t>
   </si>
   <si>
@@ -349,12 +346,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>TỔNG CỘNG (KIỆN):</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tổng số tiền phải thu: </t>
-  </si>
-  <si>
     <t>đ</t>
   </si>
   <si>
@@ -362,6 +353,27 @@
   </si>
   <si>
     <t>Người lập</t>
+  </si>
+  <si>
+    <t>Loại xe: ${nguoiGui.fullName}</t>
+  </si>
+  <si>
+    <t>Biển số xe:${nguoiGui.fullName}</t>
+  </si>
+  <si>
+    <t>Ngày chạy:${nguoiGui.fullName}</t>
+  </si>
+  <si>
+    <t>STT</t>
+  </si>
+  <si>
+    <t>Nhà xe:${nguoiGui.fullName}</t>
+  </si>
+  <si>
+    <t>TỔNG CỘNG (KIỆN):${nguoiGui.fullName}</t>
+  </si>
+  <si>
+    <t>Tổng số tiền phải thu: ${nguoiGui.fullName}</t>
   </si>
   <si>
     <r>
@@ -375,7 +387,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>${nguoiGui.fullName}</t>
+      <t>${vtToaHang.toaHangCode}</t>
     </r>
   </si>
   <si>
@@ -390,17 +402,8 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>${nguoiGui.fullName}</t>
-    </r>
-  </si>
-  <si>
-    <t>Loại xe: ${nguoiGui.fullName}</t>
-  </si>
-  <si>
-    <t>Biển số xe:${nguoiGui.fullName}</t>
-  </si>
-  <si>
-    <t>Ngày chạy:${nguoiGui.fullName}</t>
+      <t>${ngayLap}</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -588,7 +591,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -641,9 +644,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -653,15 +653,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -670,9 +661,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -694,18 +682,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -714,11 +690,29 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -797,15 +791,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>64477</xdr:colOff>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1030816</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>385314</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>122765</xdr:rowOff>
+      <xdr:rowOff>151340</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -828,8 +822,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="64477" y="0"/>
-          <a:ext cx="966339" cy="694265"/>
+          <a:off x="9525" y="28575"/>
+          <a:ext cx="966339" cy="732365"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1126,54 +1120,54 @@
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="28" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
     </row>
     <row r="2" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="29" t="s">
+      <c r="A2" s="25"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
       <c r="G4" s="4"/>
       <c r="H4" s="5" t="s">
         <v>8</v>
@@ -1184,11 +1178,11 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
       <c r="G5" s="4"/>
       <c r="H5" s="5" t="s">
         <v>9</v>
@@ -1199,11 +1193,11 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
       <c r="G6" s="4"/>
       <c r="H6" s="5" t="s">
         <v>17</v>
@@ -1426,260 +1420,244 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="F5" sqref="F5:L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" customWidth="1"/>
-    <col min="9" max="9" width="23.42578125" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" customWidth="1"/>
-    <col min="13" max="13" width="24.85546875" customWidth="1"/>
-    <col min="14" max="14" width="13.42578125" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" customWidth="1"/>
-    <col min="16" max="16" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" customWidth="1"/>
+    <col min="14" max="14" width="24.85546875" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" customWidth="1"/>
+    <col min="17" max="17" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="32" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="28"/>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="31" t="s">
+    <row r="1" spans="1:17" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+    </row>
+    <row r="2" spans="1:17" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+    </row>
+    <row r="3" spans="1:17" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F3" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+    </row>
+    <row r="4" spans="1:17" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+    </row>
+    <row r="5" spans="1:17" s="28" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="F5" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="48"/>
+    </row>
+    <row r="6" spans="1:17" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="G6" s="31"/>
+    </row>
+    <row r="7" spans="1:17" s="28" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="32"/>
+      <c r="D7" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" s="49"/>
+      <c r="H7" s="50" t="s">
+        <v>65</v>
+      </c>
+      <c r="I7" s="50"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+    </row>
+    <row r="8" spans="1:17" s="28" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="32"/>
+      <c r="H8" s="35"/>
+      <c r="J8" s="31"/>
+    </row>
+    <row r="9" spans="1:17" s="28" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-    </row>
-    <row r="2" spans="1:16" s="32" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-    </row>
-    <row r="3" spans="1:16" s="32" customFormat="1" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E3" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-    </row>
-    <row r="4" spans="1:16" s="32" customFormat="1" ht="16.149999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-    </row>
-    <row r="5" spans="1:16" s="32" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="E5" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
-    </row>
-    <row r="6" spans="1:16" s="32" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="33"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="F6" s="36"/>
-    </row>
-    <row r="7" spans="1:16" s="32" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="37" t="s">
+      <c r="B9" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="37"/>
-      <c r="C7" s="53" t="s">
+      <c r="C9" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="J9" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="K9" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="L9" s="36" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" s="28" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="D11" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="O11" s="33"/>
+      <c r="P11" s="29"/>
+      <c r="Q11" s="29"/>
+    </row>
+    <row r="12" spans="1:17" s="43" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53" t="s">
+      <c r="C12" s="51"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="F7" s="53"/>
-      <c r="G7" s="54" t="s">
-        <v>70</v>
-      </c>
-      <c r="H7" s="54"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="39"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-    </row>
-    <row r="8" spans="1:16" s="32" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="37"/>
-      <c r="G8" s="40"/>
-      <c r="I8" s="36"/>
-    </row>
-    <row r="9" spans="1:16" s="32" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="41" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="G9" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="H9" s="41" t="s">
-        <v>57</v>
-      </c>
-      <c r="I9" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="J9" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="K9" s="41" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="43"/>
-      <c r="B10" s="43"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="43"/>
-    </row>
-    <row r="11" spans="1:16" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="43"/>
-      <c r="B11" s="43"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="43"/>
-    </row>
-    <row r="12" spans="1:16" s="32" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="45"/>
-      <c r="B12" s="46"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="48"/>
-      <c r="J12" s="46"/>
-      <c r="K12" s="46"/>
-    </row>
-    <row r="13" spans="1:16" s="32" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="C13" s="32" t="s">
+      <c r="I12" s="49"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="N13" s="38"/>
-      <c r="O13" s="33"/>
-      <c r="P13" s="33"/>
-    </row>
-    <row r="14" spans="1:16" s="52" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A14" s="49" t="s">
+      <c r="L12" s="32"/>
+    </row>
+    <row r="13" spans="1:17" s="28" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="B13" s="40"/>
+    </row>
+    <row r="14" spans="1:17" s="28" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="32"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="50" t="s">
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="I14" s="51"/>
-      <c r="J14" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="K14" s="37"/>
-    </row>
-    <row r="15" spans="1:16" s="32" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A15" s="49"/>
-    </row>
-    <row r="16" spans="1:16" s="32" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A16" s="40"/>
-      <c r="B16" s="40"/>
-      <c r="C16" s="40" t="s">
-        <v>64</v>
-      </c>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40" t="s">
-        <v>65</v>
-      </c>
-      <c r="J16" s="40"/>
-      <c r="K16" s="40"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="E1:K1"/>
-    <mergeCell ref="E2:K2"/>
-    <mergeCell ref="E3:K3"/>
-    <mergeCell ref="E5:K5"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
+  <mergeCells count="10">
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="B1:D2"/>
+    <mergeCell ref="F1:L1"/>
+    <mergeCell ref="F2:L2"/>
+    <mergeCell ref="F3:L3"/>
+    <mergeCell ref="F5:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
fix cac comment khach hang
</commit_message>
<xml_diff>
--- a/src/main/resources/fileTemplate/templatePhieuBienNhan.xlsx
+++ b/src/main/resources/fileTemplate/templatePhieuBienNhan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Ghi chú</t>
   </si>
@@ -33,9 +33,6 @@
     <t>${item.numbers}</t>
   </si>
   <si>
-    <t>${item.cost}</t>
-  </si>
-  <si>
     <t xml:space="preserve">CÔNG TY TNHH GIAO NHẬN &amp; VẬN TẢI TỐC ĐỘ VIỆT NAM </t>
   </si>
   <si>
@@ -67,9 +64,6 @@
   </si>
   <si>
     <t>Số HĐ</t>
-  </si>
-  <si>
-    <t>GTN</t>
   </si>
   <si>
     <t>Số tiền phải thu</t>
@@ -205,6 +199,18 @@
       </rPr>
       <t>${vtToaHang.toaHangCode}</t>
     </r>
+  </si>
+  <si>
+    <t>${item.soHopDong}</t>
+  </si>
+  <si>
+    <t>Phiếu thu số</t>
+  </si>
+  <si>
+    <t>${item.maPhieuThu}</t>
+  </si>
+  <si>
+    <t>${item.soTienPhaiThu}</t>
   </si>
 </sst>
 </file>
@@ -334,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -374,6 +380,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -394,18 +409,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -739,7 +742,7 @@
   <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,7 +751,7 @@
     <col min="2" max="4" width="17.42578125" customWidth="1"/>
     <col min="5" max="5" width="29.28515625" customWidth="1"/>
     <col min="6" max="6" width="24.85546875" customWidth="1"/>
-    <col min="7" max="9" width="7.7109375" customWidth="1"/>
+    <col min="7" max="9" width="10.7109375" customWidth="1"/>
     <col min="10" max="10" width="17.42578125" customWidth="1"/>
     <col min="11" max="11" width="17.85546875" customWidth="1"/>
     <col min="12" max="12" width="15.5703125" customWidth="1"/>
@@ -760,49 +763,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="2" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
       <c r="E1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+    </row>
+    <row r="2" spans="1:17" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-    </row>
-    <row r="2" spans="1:17" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" s="23" t="s">
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+    </row>
+    <row r="3" spans="1:17" s="2" customFormat="1" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F3" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-    </row>
-    <row r="3" spans="1:17" s="2" customFormat="1" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F3" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
     </row>
     <row r="4" spans="1:17" s="2" customFormat="1" ht="16.149999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="F4" s="3"/>
@@ -814,15 +817,15 @@
       <c r="L4" s="3"/>
     </row>
     <row r="5" spans="1:17" s="2" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="F5" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
+      <c r="F5" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
     </row>
     <row r="6" spans="1:17" s="2" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="3"/>
@@ -833,24 +836,24 @@
     </row>
     <row r="7" spans="1:17" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="16"/>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20" t="s">
+      <c r="G7" s="23"/>
+      <c r="H7" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="20"/>
-      <c r="H7" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
       <c r="L7" s="18"/>
       <c r="M7" s="3"/>
     </row>
@@ -861,79 +864,83 @@
     </row>
     <row r="9" spans="1:17" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B9" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="D9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="E9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="F9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="G9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="H9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="I9" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9" s="10" t="s">
         <v>15</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>17</v>
       </c>
       <c r="K9" s="9" t="s">
         <v>0</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:17" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="E10" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="F10" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="K10" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="L10" s="19" t="s">
         <v>27</v>
-      </c>
-      <c r="F10" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="G10" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="K10" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="L10" s="26" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:17" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="D11" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="O11" s="7"/>
       <c r="P11" s="3"/>
@@ -941,24 +948,24 @@
     </row>
     <row r="12" spans="1:17" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>30</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>32</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="13"/>
-      <c r="F12" s="19" t="s">
+      <c r="F12" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="17" t="s">
-        <v>33</v>
-      </c>
       <c r="K12" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L12" s="6"/>
     </row>
@@ -969,13 +976,13 @@
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="I14" s="8"/>
       <c r="J14" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>

</xml_diff>